<commit_message>
Opening Excel And Inward Code Change By Dharmesh And Trigger Change Dt : 31-01-2023 Time : 20:05
</commit_message>
<xml_diff>
--- a/SUNMark/wwwroot/openingstockcoil.xlsx
+++ b/SUNMark/wwwroot/openingstockcoil.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="17175" windowHeight="9225"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="15600" windowHeight="9225"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>INWARD DATE</t>
   </si>
@@ -58,13 +58,19 @@
   </si>
   <si>
     <t>SIZE</t>
+  </si>
+  <si>
+    <t>COIL PREFIX</t>
+  </si>
+  <si>
+    <t>SUFIX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +172,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -244,6 +255,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -278,6 +290,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -453,32 +466,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,31 +508,37 @@
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -528,24 +548,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Inward, Coil Stock Excel Code Change By Dharmesh Dt : 09-02-2023 Time : 10L57
</commit_message>
<xml_diff>
--- a/SUNMark/wwwroot/openingstockcoil.xlsx
+++ b/SUNMark/wwwroot/openingstockcoil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>INWARD DATE</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>SUFIX</t>
+  </si>
+  <si>
+    <t>PRODUCT</t>
+  </si>
+  <si>
+    <t>COIL TYPE</t>
   </si>
 </sst>
 </file>
@@ -101,7 +107,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -124,11 +130,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -164,6 +181,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -467,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +512,7 @@
     <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,6 +560,12 @@
       </c>
       <c r="P1" s="12" t="s">
         <v>11</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code Change Open Excel On Dharmesh Dt : 09-05-2023
</commit_message>
<xml_diff>
--- a/SUNMark/wwwroot/openingstockcoil.xlsx
+++ b/SUNMark/wwwroot/openingstockcoil.xlsx
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>